<commit_message>
If the precursor m/z from MSP is different from m/z from CSF file, then the precursor m/z from MSP if used.
</commit_message>
<xml_diff>
--- a/src/main/resources/org/dulab/adapcompounddb/site/services/io/export_template.xlsx
+++ b/src/main/resources/org/dulab/adapcompounddb/site/services/io/export_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aleksandrsmirnov/Projects/adap/adap-kdb/src/main/resources/org/dulab/adapcompounddb/site/services/io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67E3BD7-34E1-A34A-B570-173E7C55DAFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53F99B6-A019-E741-A4E9-10B7E53EA994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1520" yWindow="500" windowWidth="44120" windowHeight="26600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -243,30 +243,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -275,6 +251,30 @@
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCD"/>
+        <bgColor indexed="9"/>
       </patternFill>
     </fill>
   </fills>
@@ -347,73 +347,73 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,6 +422,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCCFFCD"/>
+      <color rgb="FFFFFF99"/>
+      <color rgb="FFCCFFFF"/>
       <color rgb="FFD0E1E7"/>
       <color rgb="FF76D8E4"/>
       <color rgb="FFBDD8E4"/>
@@ -738,7 +741,7 @@
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -759,7 +762,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="3"/>
@@ -772,234 +775,234 @@
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:3" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="31" t="s">
+    <row r="7" spans="1:3" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="31"/>
-      <c r="B8" s="15" t="s">
+    <row r="8" spans="1:3" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="13"/>
+      <c r="B8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="31"/>
-      <c r="B9" s="23" t="s">
+    <row r="9" spans="1:3" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="13"/>
+      <c r="B9" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="32" t="s">
+    <row r="10" spans="1:3" s="17" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="32"/>
-      <c r="B11" s="9" t="s">
+    <row r="11" spans="1:3" s="17" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="14"/>
+      <c r="B11" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="16" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="32"/>
-      <c r="B12" s="9" t="s">
+    <row r="12" spans="1:3" s="17" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="14"/>
+      <c r="B12" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="32"/>
-      <c r="B13" s="24" t="s">
+    <row r="13" spans="1:3" s="17" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="14"/>
+      <c r="B13" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="16" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="32"/>
-      <c r="B14" s="9" t="s">
+    <row r="14" spans="1:3" s="17" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="14"/>
+      <c r="B14" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="16" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="32"/>
-      <c r="B15" s="9" t="s">
+    <row r="15" spans="1:3" s="17" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="14"/>
+      <c r="B15" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="28" t="s">
+    <row r="16" spans="1:3" s="22" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="29"/>
-      <c r="B17" s="33" t="s">
+    <row r="17" spans="1:3" s="22" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="23"/>
+      <c r="B17" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="21" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="7" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A18" s="29"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="20" t="s">
+    <row r="18" spans="1:3" s="22" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" s="23"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="7" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A19" s="29"/>
-      <c r="B19" s="6" t="s">
+    <row r="19" spans="1:3" s="22" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" s="23"/>
+      <c r="B19" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="21" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="29"/>
-      <c r="B20" s="6" t="s">
+    <row r="20" spans="1:3" s="22" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="23"/>
+      <c r="B20" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="21" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="7" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A21" s="29"/>
-      <c r="B21" s="33" t="s">
+    <row r="21" spans="1:3" s="22" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A21" s="23"/>
+      <c r="B21" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="21" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="29"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="20" t="s">
+    <row r="22" spans="1:3" s="22" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="23"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="21" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="29"/>
-      <c r="B23" s="6" t="s">
+    <row r="23" spans="1:3" s="22" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="23"/>
+      <c r="B23" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="30"/>
-      <c r="B24" s="6" t="s">
+    <row r="24" spans="1:3" s="22" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="26"/>
+      <c r="B24" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="21" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="25" t="s">
+    <row r="25" spans="1:3" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="21" t="s">
+      <c r="C25" s="29" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="26"/>
-      <c r="B26" s="4" t="s">
+    <row r="26" spans="1:3" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="31"/>
+      <c r="B26" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="29" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="26"/>
-      <c r="B27" s="4" t="s">
+    <row r="27" spans="1:3" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="31"/>
+      <c r="B27" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="29" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="26"/>
-      <c r="B28" s="4" t="s">
+    <row r="28" spans="1:3" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="31"/>
+      <c r="B28" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="C28" s="29" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="26"/>
-      <c r="B29" s="8" t="s">
+    <row r="29" spans="1:3" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="31"/>
+      <c r="B29" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="C29" s="29" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="27"/>
-      <c r="B30" s="13" t="s">
+    <row r="30" spans="1:3" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="33"/>
+      <c r="B30" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C30" s="29" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="17" t="s">
+    <row r="31" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="11" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modify the Excel template
</commit_message>
<xml_diff>
--- a/src/main/resources/org/dulab/adapcompounddb/site/services/io/export_template.xlsx
+++ b/src/main/resources/org/dulab/adapcompounddb/site/services/io/export_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aleksandrsmirnov/Projects/adap/adap-kdb/src/main/resources/org/dulab/adapcompounddb/site/services/io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B844FBE5-CDE0-234F-9F6F-986B98FCB33F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DD092A-DAF4-E242-A3B3-FA67C2AA2BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="500" windowWidth="44120" windowHeight="26600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="55000" yWindow="1080" windowWidth="44120" windowHeight="26600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -243,12 +243,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -277,6 +271,12 @@
         <bgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9900"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -347,20 +347,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -369,51 +369,51 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,6 +422,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF9900"/>
       <color rgb="FFCCFFCD"/>
       <color rgb="FFFFFF99"/>
       <color rgb="FFCCFFFF"/>
@@ -740,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -762,7 +763,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="3"/>
@@ -775,234 +776,234 @@
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:3" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="31" t="s">
+    <row r="7" spans="1:3" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="31"/>
-      <c r="B8" s="7" t="s">
+    <row r="8" spans="1:3" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="27"/>
+      <c r="B8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="31"/>
-      <c r="B9" s="12" t="s">
+    <row r="9" spans="1:3" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="27"/>
+      <c r="B9" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="32" t="s">
+    <row r="10" spans="1:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="32"/>
-      <c r="B11" s="13" t="s">
+    <row r="11" spans="1:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="28"/>
+      <c r="B11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="10" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="32"/>
-      <c r="B12" s="13" t="s">
+    <row r="12" spans="1:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="28"/>
+      <c r="B12" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="32"/>
-      <c r="B13" s="16" t="s">
+    <row r="13" spans="1:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="28"/>
+      <c r="B13" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="32"/>
-      <c r="B14" s="13" t="s">
+    <row r="14" spans="1:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="28"/>
+      <c r="B14" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="32"/>
-      <c r="B15" s="13" t="s">
+    <row r="15" spans="1:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="28"/>
+      <c r="B15" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="19" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="28" t="s">
+    <row r="16" spans="1:3" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="19" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="29"/>
-      <c r="B17" s="33" t="s">
+    <row r="17" spans="1:3" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="25"/>
+      <c r="B17" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="19" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A18" s="29"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="18" t="s">
+    <row r="18" spans="1:3" s="15" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" s="25"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="19" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A19" s="29"/>
-      <c r="B19" s="17" t="s">
+    <row r="19" spans="1:3" s="15" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" s="25"/>
+      <c r="B19" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="14" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="19" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="29"/>
-      <c r="B20" s="17" t="s">
+    <row r="20" spans="1:3" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="25"/>
+      <c r="B20" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="19" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A21" s="29"/>
-      <c r="B21" s="33" t="s">
+    <row r="21" spans="1:3" s="15" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A21" s="25"/>
+      <c r="B21" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="14" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="19" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="29"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="18" t="s">
+    <row r="22" spans="1:3" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="25"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="19" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="29"/>
-      <c r="B23" s="17" t="s">
+    <row r="23" spans="1:3" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="25"/>
+      <c r="B23" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="19" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="30"/>
-      <c r="B24" s="17" t="s">
+    <row r="24" spans="1:3" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="26"/>
+      <c r="B24" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="22" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="25" t="s">
+    <row r="25" spans="1:3" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="21" t="s">
+      <c r="C25" s="17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="22" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="26"/>
-      <c r="B26" s="20" t="s">
+    <row r="26" spans="1:3" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="22"/>
+      <c r="B26" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="17" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="22" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="26"/>
-      <c r="B27" s="20" t="s">
+    <row r="27" spans="1:3" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="22"/>
+      <c r="B27" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="17" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="22" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="26"/>
-      <c r="B28" s="20" t="s">
+    <row r="28" spans="1:3" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="22"/>
+      <c r="B28" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="C28" s="17" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="22" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="26"/>
-      <c r="B29" s="23" t="s">
+    <row r="29" spans="1:3" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="22"/>
+      <c r="B29" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="C29" s="17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="22" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="27"/>
-      <c r="B30" s="24" t="s">
+    <row r="30" spans="1:3" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="23"/>
+      <c r="B30" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C30" s="17" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="9" t="s">
+    <row r="31" spans="1:3" s="34" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="33" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1074,9 +1075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>

<commit_message>
Add CAS, HMDB, and PubChem IDs to the export and update the Excel template
</commit_message>
<xml_diff>
--- a/src/main/resources/org/dulab/adapcompounddb/site/services/io/export_template.xlsx
+++ b/src/main/resources/org/dulab/adapcompounddb/site/services/io/export_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aleksandrsmirnov/Projects/adap/adap-kdb/src/main/resources/org/dulab/adapcompounddb/site/services/io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DD092A-DAF4-E242-A3B3-FA67C2AA2BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0419D624-A257-DD47-9CF8-F9EAADB80468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="55000" yWindow="1080" windowWidth="44120" windowHeight="26600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3820" yWindow="500" windowWidth="44120" windowHeight="26600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="81">
   <si>
     <t>Simple export from ADAP-KDB</t>
   </si>
@@ -189,13 +189,88 @@
   </si>
   <si>
     <t>When data preprocessing software tool cannot provide the neutral mass for this signal, the library matching algorithm computes the neutral mass for each possible adduct. The assumed adduct that match with the measured “Precursor m/z” is listed here as the “Matching Adduct”.</t>
+  </si>
+  <si>
+    <t>CAS NO</t>
+  </si>
+  <si>
+    <t>HMDB ID</t>
+  </si>
+  <si>
+    <t>PubChem ID</t>
+  </si>
+  <si>
+    <t>CAS Registry Number</t>
+  </si>
+  <si>
+    <t>Human Metabolome Database Identifier</t>
+  </si>
+  <si>
+    <t>PubChem Identifier</t>
+  </si>
+  <si>
+    <t>Names given for each match are based on experimental or empirical data contained within the database.  These do not necessarily differentiate between isomeric forms.</t>
+  </si>
+  <si>
+    <t>Ontology Level</t>
+  </si>
+  <si>
+    <t>The following ontology levels are used to express the confidence of each match:</t>
+  </si>
+  <si>
+    <t>PD_A</t>
+  </si>
+  <si>
+    <t>OL_1</t>
+  </si>
+  <si>
+    <t>OL_2a</t>
+  </si>
+  <si>
+    <t>OL_2b</t>
+  </si>
+  <si>
+    <t>PD_B</t>
+  </si>
+  <si>
+    <t>PD_C</t>
+  </si>
+  <si>
+    <t>PD_D</t>
+  </si>
+  <si>
+    <t>Match is based on the spectral similarity, neutral mass error, and retention time error.</t>
+  </si>
+  <si>
+    <t>Matches against in-house libraries</t>
+  </si>
+  <si>
+    <t>Matches against public lirbaries</t>
+  </si>
+  <si>
+    <t>Match is based on the spectral similarity and retention time error.</t>
+  </si>
+  <si>
+    <t>Match is based on the neutral mass error and retention time error.</t>
+  </si>
+  <si>
+    <t>Match is based on the isotopic distribution similarity and neutral mass error.</t>
+  </si>
+  <si>
+    <t>Match is based on the neutral mass error only.</t>
+  </si>
+  <si>
+    <t>Match is based on the spectral similarity and neutral mass error.</t>
+  </si>
+  <si>
+    <t>Match is based on the predicted spectral similarity and neutral mass error.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -232,6 +307,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -278,7 +364,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -338,11 +424,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -376,36 +471,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -414,6 +479,49 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -739,11 +847,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -757,296 +863,373 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="2" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>2</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:3" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="27" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C8" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="27"/>
-      <c r="B8" s="5" t="s">
+    <row r="9" spans="1:3" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="33"/>
+      <c r="B9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C9" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="27"/>
-      <c r="B9" s="8" t="s">
+    <row r="10" spans="1:3" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="33"/>
+      <c r="B10" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C10" s="7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="28" t="s">
+    <row r="11" spans="1:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C11" s="10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="28"/>
-      <c r="B11" s="9" t="s">
+    <row r="12" spans="1:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="34"/>
+      <c r="B12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C12" s="10" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="28"/>
-      <c r="B12" s="9" t="s">
+    <row r="13" spans="1:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="34"/>
+      <c r="B13" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C13" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="28"/>
-      <c r="B13" s="12" t="s">
+    <row r="14" spans="1:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="34"/>
+      <c r="B14" s="12" t="s">
         <v>4</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="28"/>
-      <c r="B14" s="9" t="s">
-        <v>54</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="28"/>
+      <c r="A15" s="34"/>
       <c r="B15" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="34"/>
+      <c r="B16" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C16" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="24" t="s">
+    <row r="17" spans="1:3" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B17" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C17" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="25"/>
-      <c r="B17" s="29" t="s">
+    <row r="18" spans="1:3" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="31"/>
+      <c r="B18" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C18" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="15" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A18" s="25"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="14" t="s">
+    <row r="19" spans="1:3" s="15" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" s="31"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="15" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A19" s="25"/>
-      <c r="B19" s="13" t="s">
+    <row r="20" spans="1:3" s="15" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" s="31"/>
+      <c r="B20" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C20" s="14" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="25"/>
-      <c r="B20" s="13" t="s">
+    <row r="21" spans="1:3" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="31"/>
+      <c r="B21" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C21" s="14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="15" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A21" s="25"/>
-      <c r="B21" s="29" t="s">
+    <row r="22" spans="1:3" s="15" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A22" s="31"/>
+      <c r="B22" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C22" s="14" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="25"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="14" t="s">
+    <row r="23" spans="1:3" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="31"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="25"/>
-      <c r="B23" s="13" t="s">
+    <row r="24" spans="1:3" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="31"/>
+      <c r="B24" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C24" s="14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="26"/>
-      <c r="B24" s="13" t="s">
+    <row r="25" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="31"/>
+      <c r="B25" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="14"/>
+    </row>
+    <row r="26" spans="1:3" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="32"/>
+      <c r="B26" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C26" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="21" t="s">
+    <row r="27" spans="1:3" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B27" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C27" s="17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="22"/>
-      <c r="B26" s="16" t="s">
+    <row r="28" spans="1:3" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="28"/>
+      <c r="B28" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C28" s="17" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="22"/>
-      <c r="B27" s="16" t="s">
+    <row r="29" spans="1:3" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="28"/>
+      <c r="B29" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C29" s="17" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="22"/>
-      <c r="B28" s="16" t="s">
+    <row r="30" spans="1:3" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="28"/>
+      <c r="B30" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C30" s="17" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="22"/>
-      <c r="B29" s="19" t="s">
+    <row r="31" spans="1:3" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="28"/>
+      <c r="B31" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C31" s="17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="23"/>
-      <c r="B30" s="20" t="s">
+    <row r="32" spans="1:3" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="28"/>
+      <c r="B32" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="28"/>
+      <c r="B33" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="28"/>
+      <c r="B34" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="29"/>
+      <c r="B35" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C35" s="17" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="34" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="31" t="s">
+    <row r="36" spans="1:3" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="32" t="s">
+      <c r="B36" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="33" t="s">
+      <c r="C36" s="23" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B35" s="1"/>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B36" s="1"/>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B37" s="1"/>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B38" s="1"/>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B39" s="1"/>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B40" s="1"/>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B41" s="1"/>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B42" s="1"/>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B43" s="1"/>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B44" s="1"/>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B45" s="1"/>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B46" s="1"/>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B47" s="1"/>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="B39" s="43"/>
+      <c r="C39" s="43"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="B40" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="C40" s="42" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="37"/>
+      <c r="B41" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41" s="39" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="37"/>
+      <c r="B42" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" s="39" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="39" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="37"/>
+      <c r="B44" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="C44" s="39" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="37"/>
+      <c r="B45" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="C45" s="39" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="37"/>
+      <c r="B46" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C46" s="39" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C47" s="1"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B48" s="1"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.2">
@@ -1055,17 +1238,34 @@
     <row r="50" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B50" s="1"/>
     </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B51" s="1"/>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B52" s="1"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B53" s="1"/>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B54" s="1"/>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B55" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A25:A30"/>
-    <mergeCell ref="A16:A24"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A10:A15"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B21:B22"/>
+  <mergeCells count="8">
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="A27:A35"/>
+    <mergeCell ref="A17:A26"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A16"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B22:B23"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A3" location="'Data'!A1" display="Click here to see results" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A4" location="'Data'!A1" display="Click here to see results" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add InChI Key to the export
</commit_message>
<xml_diff>
--- a/src/main/resources/org/dulab/adapcompounddb/site/services/io/export_template.xlsx
+++ b/src/main/resources/org/dulab/adapcompounddb/site/services/io/export_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aleksandrsmirnov/Projects/adap/adap-kdb/src/main/resources/org/dulab/adapcompounddb/site/services/io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0419D624-A257-DD47-9CF8-F9EAADB80468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6629170D-7105-D64F-BF84-FACD6E2FC93B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3820" yWindow="500" windowWidth="44120" windowHeight="26600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
   <si>
     <t>Simple export from ADAP-KDB</t>
   </si>
@@ -264,6 +264,12 @@
   </si>
   <si>
     <t>Match is based on the predicted spectral similarity and neutral mass error.</t>
+  </si>
+  <si>
+    <t>InChI Key</t>
+  </si>
+  <si>
+    <t>International Chemical Identifier (InChI) Key</t>
   </si>
 </sst>
 </file>
@@ -481,47 +487,47 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -847,7 +853,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
@@ -888,7 +894,7 @@
       <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="40" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -899,7 +905,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="33"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="5" t="s">
         <v>11</v>
       </c>
@@ -908,7 +914,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="33"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="8" t="s">
         <v>50</v>
       </c>
@@ -917,7 +923,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="41" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -928,7 +934,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="34"/>
+      <c r="A12" s="41"/>
       <c r="B12" s="9" t="s">
         <v>13</v>
       </c>
@@ -937,7 +943,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="34"/>
+      <c r="A13" s="41"/>
       <c r="B13" s="9" t="s">
         <v>3</v>
       </c>
@@ -946,7 +952,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="34"/>
+      <c r="A14" s="41"/>
       <c r="B14" s="12" t="s">
         <v>4</v>
       </c>
@@ -955,7 +961,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="34"/>
+      <c r="A15" s="41"/>
       <c r="B15" s="9" t="s">
         <v>54</v>
       </c>
@@ -964,7 +970,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="34"/>
+      <c r="A16" s="41"/>
       <c r="B16" s="9" t="s">
         <v>15</v>
       </c>
@@ -973,7 +979,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="37" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="13" t="s">
@@ -984,8 +990,8 @@
       </c>
     </row>
     <row r="18" spans="1:3" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="31"/>
-      <c r="B18" s="35" t="s">
+      <c r="A18" s="38"/>
+      <c r="B18" s="42" t="s">
         <v>21</v>
       </c>
       <c r="C18" s="14" t="s">
@@ -993,14 +999,14 @@
       </c>
     </row>
     <row r="19" spans="1:3" s="15" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A19" s="31"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="38"/>
+      <c r="B19" s="43"/>
       <c r="C19" s="14" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="15" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A20" s="31"/>
+      <c r="A20" s="38"/>
       <c r="B20" s="13" t="s">
         <v>24</v>
       </c>
@@ -1009,7 +1015,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="31"/>
+      <c r="A21" s="38"/>
       <c r="B21" s="13" t="s">
         <v>25</v>
       </c>
@@ -1018,8 +1024,8 @@
       </c>
     </row>
     <row r="22" spans="1:3" s="15" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A22" s="31"/>
-      <c r="B22" s="35" t="s">
+      <c r="A22" s="38"/>
+      <c r="B22" s="42" t="s">
         <v>27</v>
       </c>
       <c r="C22" s="14" t="s">
@@ -1027,14 +1033,14 @@
       </c>
     </row>
     <row r="23" spans="1:3" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="31"/>
-      <c r="B23" s="36"/>
+      <c r="A23" s="38"/>
+      <c r="B23" s="43"/>
       <c r="C23" s="14" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="31"/>
+      <c r="A24" s="38"/>
       <c r="B24" s="13" t="s">
         <v>30</v>
       </c>
@@ -1043,14 +1049,14 @@
       </c>
     </row>
     <row r="25" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="31"/>
+      <c r="A25" s="38"/>
       <c r="B25" s="13" t="s">
         <v>63</v>
       </c>
       <c r="C25" s="14"/>
     </row>
     <row r="26" spans="1:3" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="32"/>
+      <c r="A26" s="39"/>
       <c r="B26" s="13" t="s">
         <v>44</v>
       </c>
@@ -1059,7 +1065,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="27" t="s">
+      <c r="A27" s="34" t="s">
         <v>46</v>
       </c>
       <c r="B27" s="16" t="s">
@@ -1070,7 +1076,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="28"/>
+      <c r="A28" s="35"/>
       <c r="B28" s="16" t="s">
         <v>5</v>
       </c>
@@ -1079,7 +1085,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="28"/>
+      <c r="A29" s="35"/>
       <c r="B29" s="16" t="s">
         <v>34</v>
       </c>
@@ -1088,7 +1094,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="28"/>
+      <c r="A30" s="35"/>
       <c r="B30" s="16" t="s">
         <v>38</v>
       </c>
@@ -1097,7 +1103,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="28"/>
+      <c r="A31" s="35"/>
       <c r="B31" s="19" t="s">
         <v>39</v>
       </c>
@@ -1106,7 +1112,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="28"/>
+      <c r="A32" s="35"/>
       <c r="B32" s="19" t="s">
         <v>56</v>
       </c>
@@ -1115,7 +1121,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="28"/>
+      <c r="A33" s="35"/>
       <c r="B33" s="19" t="s">
         <v>57</v>
       </c>
@@ -1124,7 +1130,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="28"/>
+      <c r="A34" s="35"/>
       <c r="B34" s="19" t="s">
         <v>58</v>
       </c>
@@ -1133,104 +1139,110 @@
       </c>
     </row>
     <row r="35" spans="1:3" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="29"/>
-      <c r="B35" s="20" t="s">
+      <c r="A35" s="35"/>
+      <c r="B35" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="36"/>
+      <c r="B36" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="C36" s="17" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="21" t="s">
+    <row r="37" spans="1:3" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B36" s="22" t="s">
+      <c r="B37" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="23" t="s">
+      <c r="C37" s="23" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="43" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="B39" s="43"/>
-      <c r="C39" s="43"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="40" t="s">
+      <c r="B40" s="31"/>
+      <c r="C40" s="31"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="B40" s="41" t="s">
+      <c r="B41" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="C40" s="42" t="s">
+      <c r="C41" s="30" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="37"/>
-      <c r="B41" s="38" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="33"/>
+      <c r="B42" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="C41" s="39" t="s">
+      <c r="C42" s="28" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="37"/>
-      <c r="B42" s="38" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="33"/>
+      <c r="B43" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C42" s="39" t="s">
+      <c r="C43" s="28" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="37" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="B43" s="38" t="s">
+      <c r="B44" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="C43" s="39" t="s">
+      <c r="C44" s="28" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="37"/>
-      <c r="B44" s="38" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="33"/>
+      <c r="B45" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="C44" s="39" t="s">
+      <c r="C45" s="28" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="37"/>
-      <c r="B45" s="38" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="33"/>
+      <c r="B46" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="C45" s="39" t="s">
+      <c r="C46" s="28" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="37"/>
-      <c r="B46" s="38" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="33"/>
+      <c r="B47" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="C46" s="39" t="s">
+      <c r="C47" s="28" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C47" s="1"/>
-    </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B49" s="1"/>
@@ -1253,16 +1265,19 @@
     <row r="55" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B55" s="1"/>
     </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B56" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="A27:A35"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="A27:A36"/>
     <mergeCell ref="A17:A26"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="A11:A16"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B22:B23"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A4" location="'Data'!A1" display="Click here to see results" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>